<commit_message>
order and rename files
</commit_message>
<xml_diff>
--- a/scripts/reimputation_and_prediction/reimputation_and_prediction_data.xlsx
+++ b/scripts/reimputation_and_prediction/reimputation_and_prediction_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\proto\Desktop\tothexinxol\IRB\scripts\reimputation_and_prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F682EE86-E770-4FC1-A454-F0AC85AE6278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85862E81-40D8-480E-826A-19AC185E6AA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14400" yWindow="48" windowWidth="14400" windowHeight="15600" xr2:uid="{67CED23B-338C-4776-8FD5-0AD9FF3A679A}"/>
+    <workbookView xWindow="1365" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{67CED23B-338C-4776-8FD5-0AD9FF3A679A}"/>
   </bookViews>
   <sheets>
     <sheet name="models" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="56">
   <si>
     <t>modelID</t>
   </si>
@@ -175,40 +175,25 @@
     <t>TK_FU_no3D</t>
   </si>
   <si>
-    <t>CYP450_1A2_substrate</t>
-  </si>
-  <si>
-    <t>CYP450_2C9_inhibitor</t>
-  </si>
-  <si>
-    <t>dudas</t>
-  </si>
-  <si>
-    <t>CYP450_2C19_inhibitor</t>
-  </si>
-  <si>
-    <t>CYP450_2D6_inhibitor</t>
-  </si>
-  <si>
-    <t>CYP450_3A4_inhibitor</t>
-  </si>
-  <si>
-    <t>CYP450_3A4_substrate_NOoutliers</t>
-  </si>
-  <si>
     <t>notes</t>
   </si>
   <si>
     <t>manually_renamed EVA</t>
   </si>
   <si>
-    <t>CYP450_2D6_substrate</t>
-  </si>
-  <si>
-    <t>IRB_Cavinh</t>
-  </si>
-  <si>
     <t>es no 3D</t>
+  </si>
+  <si>
+    <t>TK_BSEPinh_no3D</t>
+  </si>
+  <si>
+    <t>TK_CYP3A4sub_NOoutliers</t>
+  </si>
+  <si>
+    <t>TK_CYP2D6inh_NOoutliers</t>
+  </si>
+  <si>
+    <t>manually_renamed EVA?</t>
   </si>
 </sst>
 </file>
@@ -239,7 +224,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -264,6 +249,18 @@
         <bgColor rgb="FFC0C0C0"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor rgb="FFC0C0C0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor rgb="FFFFE699"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -277,7 +274,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -289,6 +286,11 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -606,24 +608,24 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.88671875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" customWidth="1"/>
-    <col min="8" max="8" width="19.109375" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>31</v>
@@ -644,132 +646,131 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C9" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C10" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="7" t="s">
         <v>32</v>
-      </c>
-      <c r="D15" t="s">
-        <v>29</v>
       </c>
       <c r="E15" t="s">
         <v>29</v>
@@ -784,65 +785,70 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C20" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>21</v>
       </c>
@@ -850,24 +856,26 @@
       <c r="C24" s="3"/>
       <c r="J24" s="6"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4" t="s">
+      <c r="B25" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="9" t="s">
         <v>48</v>
       </c>
       <c r="D25" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B26" s="3"/>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="9" t="s">
         <v>33</v>
       </c>
       <c r="D26" t="s">
@@ -886,32 +894,32 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>27</v>
       </c>
       <c r="D30" t="s">
         <v>29</v>
@@ -930,12 +938,12 @@
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>35</v>
       </c>
@@ -952,7 +960,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -966,7 +974,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>

</xml_diff>

<commit_message>
rename and oorder files
</commit_message>
<xml_diff>
--- a/scripts/reimputation_and_prediction/reimputation_and_prediction_data.xlsx
+++ b/scripts/reimputation_and_prediction/reimputation_and_prediction_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\proto\Desktop\tothexinxol\IRB\scripts\reimputation_and_prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9B84BAD-8651-44E9-9C1B-8686C4651ACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95457BA2-24A6-406A-8CD2-942AF6F152CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="570" yWindow="1380" windowWidth="21600" windowHeight="11385" xr2:uid="{67CED23B-338C-4776-8FD5-0AD9FF3A679A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{67CED23B-338C-4776-8FD5-0AD9FF3A679A}"/>
   </bookViews>
   <sheets>
     <sheet name="models" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="65">
   <si>
     <t>modelID</t>
   </si>
@@ -82,12 +82,6 @@
     <t>TK_HIA</t>
   </si>
   <si>
-    <t>TK_pgpinh</t>
-  </si>
-  <si>
-    <t>TK_pgpsub</t>
-  </si>
-  <si>
     <t>TK_logKp</t>
   </si>
   <si>
@@ -190,10 +184,43 @@
     <t>TK_CYP3A4sub_NOoutliers</t>
   </si>
   <si>
-    <t>TK_CYP2D6inh_NOoutliers</t>
-  </si>
-  <si>
     <t>manually_renamed EVA?</t>
+  </si>
+  <si>
+    <t>TK_CYP1A2sub_NOoutliers</t>
+  </si>
+  <si>
+    <t>TK_CYP2C9sub_NOoutliers_us</t>
+  </si>
+  <si>
+    <t>TK_CYP2C19sub_NOoutliers_us</t>
+  </si>
+  <si>
+    <t>TK_CYP2D6inh_NOoutliers_us</t>
+  </si>
+  <si>
+    <t>TK_CYP2D6sub_NOoutliers</t>
+  </si>
+  <si>
+    <t>TK_HIA_us</t>
+  </si>
+  <si>
+    <t>TK_HLM_us</t>
+  </si>
+  <si>
+    <t>TK_OATP1B3inh_no3D_us</t>
+  </si>
+  <si>
+    <t>TK_Pgpinh</t>
+  </si>
+  <si>
+    <t>TK_Pgpsub</t>
+  </si>
+  <si>
+    <t>TOX_hERGinh_NOoutliers</t>
+  </si>
+  <si>
+    <t>TOX_Nav15inh_NOoutliers_no3D_us</t>
   </si>
 </sst>
 </file>
@@ -251,13 +278,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFC0C0C0"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFE699"/>
       </patternFill>
     </fill>
@@ -607,8 +634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C412ED3-1946-48B3-A8DC-FD241BBA4E79}">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,35 +652,47 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -661,10 +700,19 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -672,10 +720,19 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>2</v>
+        <v>54</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -683,10 +740,19 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>3</v>
+        <v>55</v>
+      </c>
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -694,10 +760,19 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>4</v>
+        <v>53</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -705,10 +780,19 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>5</v>
+        <v>57</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -718,16 +802,34 @@
       <c r="C9" s="7" t="s">
         <v>6</v>
       </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -735,18 +837,36 @@
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="7" t="s">
         <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" t="s">
+        <v>27</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -754,32 +874,56 @@
         <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>54</v>
+        <v>56</v>
+      </c>
+      <c r="D13" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" t="s">
+        <v>27</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="C14" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" t="s">
+        <v>27</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="D15" t="s">
+        <v>27</v>
       </c>
       <c r="E15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H15">
         <v>1</v>
@@ -790,7 +934,16 @@
         <v>13</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>32</v>
+        <v>60</v>
+      </c>
+      <c r="D16" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16" t="s">
+        <v>27</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -798,10 +951,19 @@
         <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="7" t="s">
-        <v>52</v>
+      <c r="D17" t="s">
+        <v>27</v>
+      </c>
+      <c r="G17" t="s">
+        <v>27</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -809,86 +971,167 @@
         <v>15</v>
       </c>
       <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" t="s">
+        <v>27</v>
+      </c>
+      <c r="G18" t="s">
+        <v>27</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
+      <c r="C19" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" t="s">
+        <v>27</v>
+      </c>
+      <c r="G19" t="s">
+        <v>27</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B20" s="3"/>
-      <c r="C20" s="3" t="s">
-        <v>17</v>
+      <c r="C20" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" t="s">
+        <v>27</v>
+      </c>
+      <c r="G20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>18</v>
+        <v>61</v>
       </c>
       <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" t="s">
+        <v>27</v>
+      </c>
+      <c r="G21" t="s">
+        <v>27</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>19</v>
+        <v>62</v>
       </c>
       <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
+      <c r="C22" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22" t="s">
+        <v>27</v>
+      </c>
+      <c r="G22" t="s">
+        <v>27</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
+      <c r="C23" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" t="s">
+        <v>27</v>
+      </c>
+      <c r="G23" t="s">
+        <v>27</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
+      <c r="C24" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" t="s">
+        <v>27</v>
+      </c>
+      <c r="G24" t="s">
+        <v>27</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
       <c r="J24" s="6"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D25" t="s">
-        <v>29</v>
+        <v>27</v>
+      </c>
+      <c r="G25" t="s">
+        <v>27</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D26" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E26" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F26" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G26" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H26">
         <v>1</v>
@@ -896,36 +1139,74 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
+      <c r="C27" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G27" t="s">
+        <v>27</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>25</v>
+        <v>63</v>
+      </c>
+      <c r="D28" t="s">
+        <v>27</v>
+      </c>
+      <c r="G28" t="s">
+        <v>27</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D29" t="s">
+        <v>27</v>
+      </c>
+      <c r="G29" t="s">
+        <v>27</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D30" t="s">
-        <v>29</v>
+        <v>27</v>
+      </c>
+      <c r="G30" t="s">
+        <v>27</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -948,50 +1229,50 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
         <v>42</v>
       </c>
-      <c r="C1" t="s">
-        <v>44</v>
-      </c>
       <c r="D1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix lgbm colnames error
</commit_message>
<xml_diff>
--- a/scripts/reimputation_and_prediction/reimputation_and_prediction_data.xlsx
+++ b/scripts/reimputation_and_prediction/reimputation_and_prediction_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\proto\Desktop\tothexinxol\IRB\scripts\reimputation_and_prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6530285B-4616-4253-81D4-8F0EE31A18F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E96960D-ECB3-4325-A472-ABDA79F873E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{67CED23B-338C-4776-8FD5-0AD9FF3A679A}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="62">
   <si>
     <t>modelID</t>
   </si>
@@ -130,24 +130,12 @@
     <t>dataset_iD</t>
   </si>
   <si>
-    <t>me_lo_invento</t>
-  </si>
-  <si>
-    <t>me_lo_invento.txt</t>
-  </si>
-  <si>
-    <t>me_lo_invento2</t>
-  </si>
-  <si>
     <t>calculate</t>
   </si>
   <si>
     <t>\t</t>
   </si>
   <si>
-    <t>;</t>
-  </si>
-  <si>
     <t>file_to_calculate</t>
   </si>
   <si>
@@ -157,9 +145,6 @@
     <t>sep_for_calculation</t>
   </si>
   <si>
-    <t>me_lo_invento2.csv</t>
-  </si>
-  <si>
     <t>mergeJSONS</t>
   </si>
   <si>
@@ -221,6 +206,12 @@
   </si>
   <si>
     <t>TOX_Nav15inh_NOoutliers_no3D_us</t>
+  </si>
+  <si>
+    <t>TOX_Nav15inh_NOoutliers_no3D_us-descriptors-test.txt</t>
+  </si>
+  <si>
+    <t>TOX_Nav15inh_topredict</t>
   </si>
 </sst>
 </file>
@@ -301,7 +292,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -318,6 +309,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -635,7 +627,7 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -652,7 +644,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>29</v>
@@ -664,18 +656,18 @@
         <v>28</v>
       </c>
       <c r="F1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="H1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -685,6 +677,9 @@
       <c r="C3" s="7" t="s">
         <v>26</v>
       </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
       <c r="G3" t="s">
         <v>27</v>
       </c>
@@ -697,10 +692,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>51</v>
+        <v>46</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
       </c>
       <c r="G4" t="s">
         <v>27</v>
@@ -714,10 +712,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>54</v>
+        <v>49</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
       </c>
       <c r="G5" t="s">
         <v>27</v>
@@ -731,10 +732,13 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>55</v>
+        <v>50</v>
+      </c>
+      <c r="D6" t="s">
+        <v>27</v>
       </c>
       <c r="G6" t="s">
         <v>27</v>
@@ -748,10 +752,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>53</v>
+      <c r="D7" t="s">
+        <v>27</v>
       </c>
       <c r="G7" t="s">
         <v>27</v>
@@ -765,10 +772,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>57</v>
+        <v>52</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
       </c>
       <c r="G8" t="s">
         <v>27</v>
@@ -784,6 +794,9 @@
       <c r="C9" s="7" t="s">
         <v>6</v>
       </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
       <c r="G9" t="s">
         <v>27</v>
       </c>
@@ -796,10 +809,13 @@
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>27</v>
       </c>
       <c r="G10" t="s">
         <v>27</v>
@@ -813,10 +829,13 @@
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>27</v>
       </c>
       <c r="G11" t="s">
         <v>27</v>
@@ -832,6 +851,9 @@
       <c r="C12" s="7" t="s">
         <v>9</v>
       </c>
+      <c r="D12" t="s">
+        <v>27</v>
+      </c>
       <c r="G12" t="s">
         <v>27</v>
       </c>
@@ -844,10 +866,13 @@
         <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>56</v>
+        <v>51</v>
+      </c>
+      <c r="D13" t="s">
+        <v>27</v>
       </c>
       <c r="G13" t="s">
         <v>27</v>
@@ -861,7 +886,10 @@
         <v>11</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>59</v>
+        <v>54</v>
+      </c>
+      <c r="D14" t="s">
+        <v>27</v>
       </c>
       <c r="G14" t="s">
         <v>27</v>
@@ -877,10 +905,7 @@
       <c r="C15" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E15" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="D15" t="s">
         <v>27</v>
       </c>
       <c r="G15" t="s">
@@ -895,7 +920,10 @@
         <v>13</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>60</v>
+        <v>55</v>
+      </c>
+      <c r="D16" t="s">
+        <v>27</v>
       </c>
       <c r="G16" t="s">
         <v>27</v>
@@ -909,10 +937,13 @@
         <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>50</v>
+        <v>45</v>
+      </c>
+      <c r="D17" t="s">
+        <v>27</v>
       </c>
       <c r="G17" t="s">
         <v>27</v>
@@ -929,6 +960,9 @@
       <c r="C18" s="9" t="s">
         <v>15</v>
       </c>
+      <c r="D18" t="s">
+        <v>27</v>
+      </c>
       <c r="G18" t="s">
         <v>27</v>
       </c>
@@ -944,6 +978,9 @@
       <c r="C19" s="9" t="s">
         <v>16</v>
       </c>
+      <c r="D19" t="s">
+        <v>27</v>
+      </c>
       <c r="G19" t="s">
         <v>27</v>
       </c>
@@ -957,7 +994,10 @@
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="9" t="s">
-        <v>58</v>
+        <v>53</v>
+      </c>
+      <c r="D20" t="s">
+        <v>27</v>
       </c>
       <c r="G20" t="s">
         <v>27</v>
@@ -968,11 +1008,14 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="9" t="s">
-        <v>61</v>
+        <v>56</v>
+      </c>
+      <c r="D21" t="s">
+        <v>27</v>
       </c>
       <c r="G21" t="s">
         <v>27</v>
@@ -983,11 +1026,14 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="9" t="s">
-        <v>62</v>
+        <v>57</v>
+      </c>
+      <c r="D22" t="s">
+        <v>27</v>
       </c>
       <c r="G22" t="s">
         <v>27</v>
@@ -1004,6 +1050,9 @@
       <c r="C23" s="9" t="s">
         <v>18</v>
       </c>
+      <c r="D23" t="s">
+        <v>27</v>
+      </c>
       <c r="G23" t="s">
         <v>27</v>
       </c>
@@ -1019,6 +1068,9 @@
       <c r="C24" s="9" t="s">
         <v>19</v>
       </c>
+      <c r="D24" t="s">
+        <v>27</v>
+      </c>
       <c r="G24" t="s">
         <v>27</v>
       </c>
@@ -1032,10 +1084,13 @@
         <v>20</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>46</v>
+        <v>41</v>
+      </c>
+      <c r="D25" t="s">
+        <v>27</v>
       </c>
       <c r="G25" t="s">
         <v>27</v>
@@ -1052,10 +1107,7 @@
       <c r="C26" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E26" t="s">
-        <v>27</v>
-      </c>
-      <c r="F26" t="s">
+      <c r="D26" t="s">
         <v>27</v>
       </c>
       <c r="G26" t="s">
@@ -1073,6 +1125,9 @@
       <c r="C27" s="7" t="s">
         <v>22</v>
       </c>
+      <c r="D27" t="s">
+        <v>27</v>
+      </c>
       <c r="G27" t="s">
         <v>27</v>
       </c>
@@ -1085,39 +1140,45 @@
         <v>23</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D28" t="s">
         <v>27</v>
       </c>
-      <c r="G28" t="s">
-        <v>27</v>
-      </c>
+      <c r="G28" s="6"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="G29" t="s">
-        <v>27</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G29" s="6"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G30" t="s">
-        <v>27</v>
-      </c>
+      <c r="D30" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G30" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1126,15 +1187,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A07B663-65BB-4F15-95F1-F8014A88D2EB}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="23" customWidth="1"/>
+    <col min="1" max="1" width="42.140625" customWidth="1"/>
+    <col min="2" max="2" width="54.28515625" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1142,13 +1205,13 @@
         <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E1" t="s">
         <v>28</v>
@@ -1156,34 +1219,23 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" t="s">
         <v>35</v>
       </c>
-      <c r="C2" t="s">
-        <v>38</v>
+      <c r="D2" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" t="s">
-        <v>27</v>
-      </c>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E8" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Revert "Merge branch 'main' of https://github.com/ProtoQSAR/IRB"
This reverts commit dd8164ff6ae33ead71e4c08f5a18db4547a3ed59, reversing
changes made to 03e8dc724b525dab0692f487169d09ad4597a3ea.
</commit_message>
<xml_diff>
--- a/scripts/reimputation_and_prediction/reimputation_and_prediction_data.xlsx
+++ b/scripts/reimputation_and_prediction/reimputation_and_prediction_data.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="133">
   <si>
     <t xml:space="preserve">modelID</t>
   </si>
@@ -50,9 +50,6 @@
     <t xml:space="preserve">batch1-merged_json</t>
   </si>
   <si>
-    <t xml:space="preserve">batch2-merged_json</t>
-  </si>
-  <si>
     <t xml:space="preserve">yes</t>
   </si>
   <si>
@@ -194,21 +191,6 @@
     <t xml:space="preserve">es no 3D</t>
   </si>
   <si>
-    <t xml:space="preserve">PhCh_logD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PhCh_logP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PhCh_MP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PhCh_BP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PhCh_WS</t>
-  </si>
-  <si>
     <t xml:space="preserve">dataset_iD</t>
   </si>
   <si>
@@ -438,12 +420,6 @@
   </si>
   <si>
     <t xml:space="preserve">input_newmodels_IRB.txt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HSI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">final_all2_for_hygieia.csv</t>
   </si>
 </sst>
 </file>
@@ -513,13 +489,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.3997"/>
+        <fgColor theme="7" tint="0.3998"/>
         <bgColor rgb="FFFFFF99"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.3997"/>
+        <fgColor theme="4" tint="0.3998"/>
         <bgColor rgb="FFA6A6A6"/>
       </patternFill>
     </fill>
@@ -852,22 +828,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E32" activeCellId="1" sqref="E38 E32"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="1" sqref="D37 F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.55859375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="30.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="14.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="19.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="30.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="14.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="19.15"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -893,7 +869,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -901,212 +877,340 @@
         <v>8</v>
       </c>
       <c r="E2" s="4"/>
-    </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F2" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="G3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="C4" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="H4" s="2" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="C5" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="H5" s="2" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="H6" s="2" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="H7" s="2" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="H8" s="2" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="D9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="H9" s="2" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="B10" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="C10" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="D10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="H10" s="2" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6" t="s">
         <v>24</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>24</v>
       </c>
+      <c r="D11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="H11" s="2" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6" t="s">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>25</v>
       </c>
+      <c r="D12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="H12" s="2" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="B13" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="C13" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="H13" s="2" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="H14" s="2" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="H15" s="2" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="H16" s="2" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="H17" s="2" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="5" t="s">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="7" t="s">
         <v>36</v>
       </c>
+      <c r="B18" s="7"/>
+      <c r="C18" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
       <c r="H18" s="2" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="7" t="s">
         <v>37</v>
       </c>
@@ -1114,35 +1218,63 @@
       <c r="C19" s="8" t="s">
         <v>37</v>
       </c>
+      <c r="D19" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="H19" s="2" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="7" t="s">
         <v>38</v>
       </c>
       <c r="B20" s="7"/>
       <c r="C20" s="8" t="s">
-        <v>38</v>
+        <v>39</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="H20" s="2" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B21" s="7"/>
       <c r="C21" s="8" t="s">
         <v>40</v>
       </c>
+      <c r="D21" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="H21" s="2" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="7" t="s">
         <v>41</v>
       </c>
@@ -1150,11 +1282,21 @@
       <c r="C22" s="8" t="s">
         <v>41</v>
       </c>
+      <c r="D22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="H22" s="2" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="7" t="s">
         <v>42</v>
       </c>
@@ -1162,11 +1304,21 @@
       <c r="C23" s="8" t="s">
         <v>42</v>
       </c>
+      <c r="D23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="H23" s="2" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="7" t="s">
         <v>43</v>
       </c>
@@ -1174,189 +1326,153 @@
       <c r="C24" s="8" t="s">
         <v>43</v>
       </c>
+      <c r="D24" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="H24" s="2" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="7" t="s">
+      <c r="J24" s="4"/>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B25" s="7"/>
+      <c r="B25" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="C25" s="8" t="s">
-        <v>44</v>
+        <v>46</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="H25" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="J25" s="4"/>
-    </row>
-    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>46</v>
-      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="7"/>
       <c r="C26" s="8" t="s">
-        <v>47</v>
+        <v>48</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="H26" s="2" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B27" s="7"/>
-      <c r="C27" s="8" t="s">
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="10" t="s">
         <v>49</v>
       </c>
+      <c r="B27" s="10"/>
+      <c r="C27" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="H27" s="2" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="10" t="s">
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B28" s="10"/>
-      <c r="C28" s="5" t="s">
-        <v>50</v>
+      <c r="C28" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="H28" s="2" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C29" s="8" t="s">
         <v>52</v>
       </c>
+      <c r="C29" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="H29" s="2" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>54</v>
       </c>
+      <c r="D30" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="H30" s="2" t="n">
         <v>1</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="H31" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H32" s="2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H33" s="2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H34" s="2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H35" s="2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H36" s="2" t="n">
-        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1375,28 +1491,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E38" activeCellId="0" sqref="E38"/>
+      <selection pane="topLeft" activeCell="D37" activeCellId="0" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.55859375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="42.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="74.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="42.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="74.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="23"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>5</v>
@@ -1405,418 +1521,473 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C4" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C5" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="C6" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="C7" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+      <c r="C8" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
+      <c r="C9" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
+      <c r="C10" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
+      <c r="C11" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
+      <c r="C12" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
+      <c r="C13" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B14" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
+      <c r="C14" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B15" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
+      <c r="C15" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B16" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="s">
+      <c r="C16" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B17" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="s">
+      <c r="C17" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B18" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="s">
+      <c r="C18" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B19" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2" t="s">
+      <c r="C19" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B20" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2" t="s">
+      <c r="C20" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B21" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="s">
+      <c r="C21" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B22" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="s">
+      <c r="C22" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B23" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2" t="s">
+      <c r="C23" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B24" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2" t="s">
+      <c r="C24" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B25" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="2" t="s">
+      <c r="C25" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B26" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="2" t="s">
+      <c r="C26" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B27" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="2" t="s">
+      <c r="C27" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B28" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="2" t="s">
+      <c r="C28" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B29" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2" t="s">
+      <c r="C29" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B30" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="2" t="s">
+      <c r="C30" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B31" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="2" t="s">
+      <c r="C31" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B32" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="2" t="s">
+      <c r="C32" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B33" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="2" t="s">
+      <c r="C33" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B34" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="2" t="s">
+      <c r="C34" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B35" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="2" t="s">
+      <c r="C35" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B36" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="2" t="s">
+      <c r="C36" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>138</v>
-      </c>
       <c r="C37" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>10</v>
+        <v>64</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>